<commit_message>
Redirection entre index et cours sont parfaites
</commit_message>
<xml_diff>
--- a/excels/Budget Personnel.xlsx
+++ b/excels/Budget Personnel.xlsx
@@ -20,13 +20,13 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="1051">
   <si>
     <t>id</t>
   </si>
@@ -3176,17 +3176,146 @@
   </si>
   <si>
     <t>Étiquettes de lignes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">menuCours.js : import { coursContent } from "/js/coursContent.js"; // ==== MENU DEROULANT POUR LES COURS ===== const dropdownBtns = document.querySelectorAll('.dropdown-btn'); const mainCours = document.querySelector('.coursContent'); const pageTitle = document.querySelector('h1'); // ==== AFFICHER LE CONTENU ===== export function afficherContenu(id) { const cours = coursContent[id]; if (cours) { mainCours.innerHTML = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>&lt;h2&gt;${cours.title}&lt;/h2&gt; ${cours.content}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t>; } } // ==== AFFICHER LE CONTENU AU CLIC ===== dropdownBtns.forEach(btn =&gt; { btn.addEventListener('click', function (event) { event.preventDefault(); dropdownBtns.forEach(li =&gt; { li.classList.remove('active'); }); this.classList.add('active'); const id = btn.dataset.id; if (pageTitle) { pageTitle.style.display = 'none'; } if (this.classList.contains('saisie-subtheme')) { afficherContenu('saisie-simple'); } if (this.classList.contains('addition-subtheme')) { afficherContenu('additionner'); } if (this.classList.contains('manipuler-nombres-subtheme')) { afficherContenu('manipuler-nombre'); } if (this.classList.contains('moyenne-subtheme')) { afficherContenu('calculer_moyenne'); } if (this.classList.contains('valeurs-extremes-subtheme')) { afficherContenu('trouver_valeurs_extremes'); } if (this.classList.contains('traiter-dates-subtheme')) { afficherContenu('traiter_dates'); } if (this.classList.contains('compter-subtheme')) { afficherContenu('compter_cellules'); } if (this.classList.contains('positions-subtheme')) { afficherContenu('utiliser-logique-position'); } if (this.classList.contains('traiter-texte-subtheme')) { afficherContenu('traiter-texte'); } if (this.classList.contains('recherche-valeur-subtheme')) { afficherContenu('recherche-valeur'); } if (this.classList.contains('operateurs-logiques-subtheme')) { afficherContenu('utiliser-operateurs-logiques'); } if (this.classList.contains('tcd-subtheme')) { afficherContenu('tableau-croise-dynamique'); } if (this.classList.contains('graph-subtheme')) { afficherContenu('graphiques'); } if (this.classList.contains('analyse-subtheme')) { afficherContenu('outils-analyse'); } if (this.classList.contains('liens-subtheme')) { afficherContenu('lier-feuilles'); } if (this.classList.contains('cellules-subtheme')) { afficherContenu('nommer-cellules'); } else { afficherContenu(id); } const targetElement = document.getElementById(id); if (targetElement) { const headerOffset = 100; const elementPosition = targetElement.getBoundingClientRect().top; const offsetPosition = elementPosition + window.pageYOffset - headerOffset; window.scrollTo({ top: offsetPosition, behavior: 'smooth' }); } else { window.scrollTo({ top: 0, behavior: 'smooth' }); } }); }); // ==== COMPORTEMENT DE L'AFFICHAGE DU MENU ===== document.addEventListener('DOMContentLoaded', function () { const toggleIcons = document.querySelectorAll('.toggle-icon'); toggleIcons.forEach(icon =&gt; { icon.addEventListener('click', function (event) { event.preventDefault(); const targetClass = this.getAttribute('data-target'); const content = document.querySelector(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.${targetClass}-content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">); const isIntroduction = targetClass === 'introduction'; const isWantToDo = targetClass === 'WantToDo'; if (content.style.display === 'none' || content.style.display === '') { content.style.display = 'block'; this.innerHTML = '&lt;ion-icon name="caret-down-outline"&gt;&lt;/ion-icon&gt;'; } else { content.style.display = 'none'; this.innerHTML = '&lt;ion-icon name="caret-forward-outline"&gt;&lt;/ion-icon&gt;'; } if (isIntroduction) { const submenus = document.querySelectorAll('.Menucontent.interface-content, .Menucontent.fichiers-content'); const subIcons = document.querySelectorAll('.interface .toggle-icon ion-icon, .fichiers .toggle-icon ion-icon'); submenus.forEach(submenu =&gt; { submenu.style.display = 'none'; }); subIcons.forEach(subIcon =&gt; { subIcon.setAttribute('name', 'caret-forward-outline'); }); } if (isWantToDo) { const submenus = document.querySelectorAll('.Menucontent.saisieDonnees-content, .Menucontent.formulesPour-content, .Menucontent.analyseDonnees-content, .Menucontent.organisationDonnees-content'); const subIcons = document.querySelectorAll('.saisieDonnees .toggle-icon ion-icon, .formulesPour .toggle-icon ion-icon, .analyseDonnees .toggle-icon ion-icon, .organisationDonnees .toggle-icon ion-icon'); submenus.forEach(submenu =&gt; { submenu.style.display = 'none'; }); subIcons.forEach(subIcon =&gt; { subIcon.setAttribute('name', 'caret-forward-outline'); }); } }); }); }); // COMPORTEMENT DE LA TAILLE DU MENU EN FONCTION DU SCROLL window.addEventListener('scroll', function() { const navCours = document.querySelector('.NavCours'); const footer = document.querySelector('footer'); const footerTop = footer.offsetTop; const scrollPosition = window.scrollY + window.innerHeight; if (scrollPosition &gt;= footerTop) { navCours.style.height = 'calc(100vh - 10vh - ' + (scrollPosition - footerTop) + 'px)'; } else { navCours.style.height = 'calc(100vh - 10vh)'; } }); main.js : // ==== SCROLL EFFECT HEADER ==== window.addEventListener("scroll", function () { const header = document.querySelector("header"); const logoHeader = document.querySelector(".logo-header img"); const logoHeaderNoir = document.querySelector(".logo-headerNoir"); const logoHeaderBlanc = document.querySelector(".logo-headerBlanc"); const links = document.querySelectorAll(".links"); const scrollPosition = window.scrollY; const headerHeight = 350; const logoHeight = 120 - (scrollPosition / headerHeight) * 30; const logoWidth = 120 - (scrollPosition / headerHeight) * 30; logoHeader.style.height = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>${logoHeight}px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">; logoHeader.style.width = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>${logoWidth}px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">; links.forEach((link) =&gt; { link.style.color = window.scrollY &gt; 250 ? "white" : "black"; }); if (window.scrollY + 10 &gt;= 250) { header.classList.add("scrolled"); logoHeader.style.transition = "all 0.3s ease-in-out"; logoHeader.style.width = "20px"; logoHeader.style.height = "auto"; logoHeaderNoir.style.display = "none"; logoHeaderBlanc.style.display = "block"; header.style.height = "8vh"; } else { header.classList.remove("scrolled"); logoHeader.style.transition = "all 0.2s ease-in-out"; logoHeader.style.height = "auto"; logoHeaderNoir.style.display = "block"; logoHeaderBlanc.style.display = "none"; header.style.height = "10vh"; } }); // ==== NAVIGATION PAGES INNER.HTML ==== window.addEventListener("DOMContentLoaded", function () { const navigation = document.getElementById("navigationPages"); const currentPageTitle = document.title; // Récupérer la page actuelle sans l'extension .html const currentPagePath = window.location.pathname.replace(/\.html$/, '').split("/").pop(); // Récupérer la page précédente enregistrée dans le localStorage const previousPage = localStorage.getItem("previousPage") || "index"; function capitalizeWords(str) { return str.replace(/\b\w/g, char =&gt; char.toUpperCase()); } let navigationChemin = ""; if (currentPageTitle === "Formation Excel") { navigationChemin += </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>Accueil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">; } else { if (previousPage) { const previousPageFormatted = previousPage === "index" ? "Accueil" : capitalizeWords(previousPage.replace(/-/g, ' ')); const previousPageLink = previousPage === "index" ? "/" : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/${previousPage}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">; navigationChemin += </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t xml:space="preserve">&lt;a href="${previousPageLink}"&gt;${previousPageFormatted}&lt;/a&gt; &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">; } navigationChemin += </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>${capitalizeWords(currentPagePath.replace(/-/g, ' '))}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="1"/>
+      </rPr>
+      <t>; } navigation.innerHTML = navigationChemin; const previousPageLink = navigation.querySelector("a"); if (previousPage &amp;&amp; currentPagePath !== "index" &amp;&amp; previousPageLink) { previousPageLink.addEventListener("click", function (event) { event.preventDefault(); window.history.back(); }); } // Enregistrer la page actuelle comme la page précédente pour la prochaine navigation localStorage.setItem("previousPage", currentPagePath); }); // ==== BUTTON DELAY ===== const delayedLinks = document.querySelectorAll('a[href$=".html"]'); delayedLinks.forEach((link) =&gt; { link.addEventListener("click", function (event) { event.preventDefault(); const url = link.getAttribute("href"); setTimeout(() =&gt; { window.location.href = url; }, 500); }); }); // ==== TEST ==== document.getElementById('buttonCoursHTML').addEventListener('click', function (event) { event.preventDefault(); localStorage.setItem('randomCourse', 'prise-en-main'); localStorage.setItem('fromIndex', 'true'); window.location.href = 'cours.html'; }); document.getElementById('formules').addEventListener('click', function (event) { event.preventDefault(); const courses = [ "additionner", "manipuler-nombre", "calculer_moyenne", "compter_cellules", "trouver_valeurs_extremes", "traiter_dates", "utiliser-operateurs-logiques", "utiliser-logique-position", "recherche-valeur" ]; const randomCourse = courses[Math.floor(Math.random() * courses.length)]; localStorage.setItem('randomCourse', randomCourse); localStorage.setItem('fromIndex', 'true'); window.location.href = 'cours.html'; }); // On vérifie si l'élément existe avant d'ajouter l'événement const buttonCoursHTML = document.getElementById('buttonCoursHTML'); if (buttonCoursHTML) { buttonCoursHTML.addEventListener('click', function (event) { event.preventDefault(); localStorage.setItem('randomCourse', 'prise-en-main'); localStorage.setItem('fromIndex', 'true'); window.location.href = 'cours.html'; }); } Voici mon globalement mon projet. J'aimerais factoriser mon code sur une partie en particulier. Dans mon code, j'ai des éléments qui permettent de faire des redirections e certaines particulières. J'aimerais rassembler et factoriser si possible les scripts visant le comportement des redirections dans un seul et même fichier JS qui s'appellera 'redirections.js'. De cette manière, les scripts intégrés dans les fichiers HTML pourront être rassemblés également dans ce même fichier</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7223,7 +7352,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:F16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField dataField="1" showAll="0"/>
@@ -7617,7 +7746,7 @@
       <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.875" bestFit="1" customWidth="1"/>
@@ -7631,7 +7760,7 @@
     <col min="11" max="11" width="16.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7666,7 +7795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7703,7 +7832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7740,7 +7869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7777,7 +7906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7814,7 +7943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7851,7 +7980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7888,7 +8017,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7925,7 +8054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7959,7 +8088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7996,7 +8125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8033,7 +8162,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
@@ -8070,7 +8199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
@@ -8107,7 +8236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>13</v>
       </c>
@@ -8144,7 +8273,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8181,7 +8310,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8218,7 +8347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8255,7 +8384,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8292,7 +8421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8329,7 +8458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8363,7 +8492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8400,7 +8529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8437,7 +8566,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8474,7 +8603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8508,7 +8637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8545,7 +8674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8579,7 +8708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>26</v>
       </c>
@@ -8616,7 +8745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>27</v>
       </c>
@@ -8653,7 +8782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>28</v>
       </c>
@@ -8690,7 +8819,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>29</v>
       </c>
@@ -8727,7 +8856,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>30</v>
       </c>
@@ -8764,7 +8893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>31</v>
       </c>
@@ -8798,7 +8927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>32</v>
       </c>
@@ -8835,7 +8964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8872,7 +9001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8906,7 +9035,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>35</v>
       </c>
@@ -8943,7 +9072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>36</v>
       </c>
@@ -8980,7 +9109,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9017,7 +9146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9051,7 +9180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>39</v>
       </c>
@@ -9088,7 +9217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>40</v>
       </c>
@@ -9125,7 +9254,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>41</v>
       </c>
@@ -9162,7 +9291,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>42</v>
       </c>
@@ -9199,7 +9328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>43</v>
       </c>
@@ -9236,7 +9365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>44</v>
       </c>
@@ -9273,7 +9402,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>45</v>
       </c>
@@ -9307,7 +9436,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>46</v>
       </c>
@@ -9344,7 +9473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>47</v>
       </c>
@@ -9381,7 +9510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>48</v>
       </c>
@@ -9415,7 +9544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>49</v>
       </c>
@@ -9452,7 +9581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>50</v>
       </c>
@@ -9489,7 +9618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>51</v>
       </c>
@@ -9526,7 +9655,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>52</v>
       </c>
@@ -9563,7 +9692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>53</v>
       </c>
@@ -9600,7 +9729,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55">
         <v>54</v>
       </c>
@@ -9637,7 +9766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56">
         <v>55</v>
       </c>
@@ -9674,7 +9803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57">
         <v>56</v>
       </c>
@@ -9711,7 +9840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58">
         <v>57</v>
       </c>
@@ -9748,7 +9877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59">
         <v>58</v>
       </c>
@@ -9782,7 +9911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60">
         <v>59</v>
       </c>
@@ -9819,7 +9948,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9853,7 +9982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62">
         <v>61</v>
       </c>
@@ -9890,7 +10019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63">
         <v>62</v>
       </c>
@@ -9924,7 +10053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64">
         <v>63</v>
       </c>
@@ -9961,7 +10090,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11">
       <c r="A65">
         <v>64</v>
       </c>
@@ -9998,7 +10127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66">
         <v>65</v>
       </c>
@@ -10035,7 +10164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11">
       <c r="A67">
         <v>66</v>
       </c>
@@ -10069,7 +10198,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68">
         <v>67</v>
       </c>
@@ -10106,7 +10235,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11">
       <c r="A69">
         <v>68</v>
       </c>
@@ -10143,7 +10272,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11">
       <c r="A70">
         <v>69</v>
       </c>
@@ -10180,7 +10309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71">
         <v>70</v>
       </c>
@@ -10217,7 +10346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72">
         <v>71</v>
       </c>
@@ -10254,7 +10383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11">
       <c r="A73">
         <v>72</v>
       </c>
@@ -10291,7 +10420,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11">
       <c r="A74">
         <v>73</v>
       </c>
@@ -10325,7 +10454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75">
         <v>74</v>
       </c>
@@ -10359,7 +10488,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76">
         <v>75</v>
       </c>
@@ -10396,7 +10525,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11">
       <c r="A77">
         <v>76</v>
       </c>
@@ -10433,7 +10562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11">
       <c r="A78">
         <v>77</v>
       </c>
@@ -10470,7 +10599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11">
       <c r="A79">
         <v>78</v>
       </c>
@@ -10504,7 +10633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11">
       <c r="A80">
         <v>79</v>
       </c>
@@ -10538,7 +10667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11">
       <c r="A81">
         <v>80</v>
       </c>
@@ -10575,7 +10704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11">
       <c r="A82">
         <v>81</v>
       </c>
@@ -10612,7 +10741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11">
       <c r="A83">
         <v>82</v>
       </c>
@@ -10649,7 +10778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11">
       <c r="A84">
         <v>83</v>
       </c>
@@ -10683,7 +10812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11">
       <c r="A85">
         <v>84</v>
       </c>
@@ -10717,7 +10846,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11">
       <c r="A86">
         <v>85</v>
       </c>
@@ -10754,7 +10883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11">
       <c r="A87">
         <v>86</v>
       </c>
@@ -10791,7 +10920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11">
       <c r="A88">
         <v>87</v>
       </c>
@@ -10828,7 +10957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11">
       <c r="A89">
         <v>88</v>
       </c>
@@ -10865,7 +10994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11">
       <c r="A90">
         <v>89</v>
       </c>
@@ -10902,7 +11031,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11">
       <c r="A91">
         <v>90</v>
       </c>
@@ -10939,7 +11068,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11">
       <c r="A92">
         <v>91</v>
       </c>
@@ -10976,7 +11105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11">
       <c r="A93">
         <v>92</v>
       </c>
@@ -11013,7 +11142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11">
       <c r="A94">
         <v>93</v>
       </c>
@@ -11050,7 +11179,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11">
       <c r="A95">
         <v>94</v>
       </c>
@@ -11087,7 +11216,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11">
       <c r="A96">
         <v>95</v>
       </c>
@@ -11121,7 +11250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11">
       <c r="A97">
         <v>96</v>
       </c>
@@ -11158,7 +11287,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11">
       <c r="A98">
         <v>97</v>
       </c>
@@ -11195,7 +11324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11">
       <c r="A99">
         <v>98</v>
       </c>
@@ -11232,7 +11361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11">
       <c r="A100">
         <v>99</v>
       </c>
@@ -11269,7 +11398,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11">
       <c r="A101">
         <v>100</v>
       </c>
@@ -11306,7 +11435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11">
       <c r="A102">
         <v>101</v>
       </c>
@@ -11343,7 +11472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11">
       <c r="A103">
         <v>102</v>
       </c>
@@ -11380,7 +11509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11">
       <c r="A104">
         <v>103</v>
       </c>
@@ -11417,7 +11546,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11">
       <c r="A105">
         <v>104</v>
       </c>
@@ -11454,7 +11583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11">
       <c r="A106">
         <v>105</v>
       </c>
@@ -11491,7 +11620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11">
       <c r="A107">
         <v>106</v>
       </c>
@@ -11525,7 +11654,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11">
       <c r="A108">
         <v>107</v>
       </c>
@@ -11559,7 +11688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11">
       <c r="A109">
         <v>108</v>
       </c>
@@ -11593,7 +11722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11">
       <c r="A110">
         <v>109</v>
       </c>
@@ -11630,7 +11759,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11">
       <c r="A111">
         <v>110</v>
       </c>
@@ -11667,7 +11796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11">
       <c r="A112">
         <v>111</v>
       </c>
@@ -11704,7 +11833,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11">
       <c r="A113">
         <v>112</v>
       </c>
@@ -11741,7 +11870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11">
       <c r="A114">
         <v>113</v>
       </c>
@@ -11778,7 +11907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11">
       <c r="A115">
         <v>114</v>
       </c>
@@ -11815,7 +11944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11">
       <c r="A116">
         <v>115</v>
       </c>
@@ -11852,7 +11981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11">
       <c r="A117">
         <v>116</v>
       </c>
@@ -11889,7 +12018,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11">
       <c r="A118">
         <v>117</v>
       </c>
@@ -11926,7 +12055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11">
       <c r="A119">
         <v>118</v>
       </c>
@@ -11960,7 +12089,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11">
       <c r="A120">
         <v>119</v>
       </c>
@@ -11994,7 +12123,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11">
       <c r="A121">
         <v>120</v>
       </c>
@@ -12031,7 +12160,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11">
       <c r="A122">
         <v>121</v>
       </c>
@@ -12068,7 +12197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11">
       <c r="A123">
         <v>122</v>
       </c>
@@ -12105,7 +12234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11">
       <c r="A124">
         <v>123</v>
       </c>
@@ -12142,7 +12271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11">
       <c r="A125">
         <v>124</v>
       </c>
@@ -12179,7 +12308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11">
       <c r="A126">
         <v>125</v>
       </c>
@@ -12213,7 +12342,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11">
       <c r="A127">
         <v>126</v>
       </c>
@@ -12250,7 +12379,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11">
       <c r="A128">
         <v>127</v>
       </c>
@@ -12287,7 +12416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11">
       <c r="A129">
         <v>128</v>
       </c>
@@ -12321,7 +12450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11">
       <c r="A130">
         <v>129</v>
       </c>
@@ -12358,7 +12487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11">
       <c r="A131">
         <v>130</v>
       </c>
@@ -12392,7 +12521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11">
       <c r="A132">
         <v>131</v>
       </c>
@@ -12429,7 +12558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11">
       <c r="A133">
         <v>132</v>
       </c>
@@ -12466,7 +12595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11">
       <c r="A134">
         <v>133</v>
       </c>
@@ -12503,7 +12632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11">
       <c r="A135">
         <v>134</v>
       </c>
@@ -12540,7 +12669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11">
       <c r="A136">
         <v>135</v>
       </c>
@@ -12577,7 +12706,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11">
       <c r="A137">
         <v>136</v>
       </c>
@@ -12614,7 +12743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11">
       <c r="A138">
         <v>137</v>
       </c>
@@ -12651,7 +12780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11">
       <c r="A139">
         <v>138</v>
       </c>
@@ -12685,7 +12814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11">
       <c r="A140">
         <v>139</v>
       </c>
@@ -12719,7 +12848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11">
       <c r="A141">
         <v>140</v>
       </c>
@@ -12756,7 +12885,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11">
       <c r="A142">
         <v>141</v>
       </c>
@@ -12793,7 +12922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11">
       <c r="A143">
         <v>142</v>
       </c>
@@ -12830,7 +12959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11">
       <c r="A144">
         <v>143</v>
       </c>
@@ -12867,7 +12996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11">
       <c r="A145">
         <v>144</v>
       </c>
@@ -12904,7 +13033,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11">
       <c r="A146">
         <v>145</v>
       </c>
@@ -12941,7 +13070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11">
       <c r="A147">
         <v>146</v>
       </c>
@@ -12978,7 +13107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11">
       <c r="A148">
         <v>147</v>
       </c>
@@ -13015,7 +13144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11">
       <c r="A149">
         <v>148</v>
       </c>
@@ -13049,7 +13178,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11">
       <c r="A150">
         <v>149</v>
       </c>
@@ -13086,7 +13215,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11">
       <c r="A151">
         <v>150</v>
       </c>
@@ -13123,7 +13252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11">
       <c r="A152">
         <v>151</v>
       </c>
@@ -13157,7 +13286,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11">
       <c r="A153">
         <v>152</v>
       </c>
@@ -13194,7 +13323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11">
       <c r="A154">
         <v>153</v>
       </c>
@@ -13231,7 +13360,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11">
       <c r="A155">
         <v>154</v>
       </c>
@@ -13268,7 +13397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11">
       <c r="A156">
         <v>155</v>
       </c>
@@ -13305,7 +13434,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11">
       <c r="A157">
         <v>156</v>
       </c>
@@ -13342,7 +13471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11">
       <c r="A158">
         <v>157</v>
       </c>
@@ -13379,7 +13508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11">
       <c r="A159">
         <v>158</v>
       </c>
@@ -13413,7 +13542,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11">
       <c r="A160">
         <v>159</v>
       </c>
@@ -13450,7 +13579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11">
       <c r="A161">
         <v>160</v>
       </c>
@@ -13484,7 +13613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11">
       <c r="A162">
         <v>161</v>
       </c>
@@ -13521,7 +13650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11">
       <c r="A163">
         <v>162</v>
       </c>
@@ -13558,7 +13687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11">
       <c r="A164">
         <v>163</v>
       </c>
@@ -13595,7 +13724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11">
       <c r="A165">
         <v>164</v>
       </c>
@@ -13632,7 +13761,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11">
       <c r="A166">
         <v>165</v>
       </c>
@@ -13669,7 +13798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11">
       <c r="A167">
         <v>166</v>
       </c>
@@ -13706,7 +13835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11">
       <c r="A168">
         <v>167</v>
       </c>
@@ -13743,7 +13872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11">
       <c r="A169">
         <v>168</v>
       </c>
@@ -13777,7 +13906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11">
       <c r="A170">
         <v>169</v>
       </c>
@@ -13814,7 +13943,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11">
       <c r="A171">
         <v>170</v>
       </c>
@@ -13848,7 +13977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11">
       <c r="A172">
         <v>171</v>
       </c>
@@ -13882,7 +14011,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11">
       <c r="A173">
         <v>172</v>
       </c>
@@ -13919,7 +14048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11">
       <c r="A174">
         <v>173</v>
       </c>
@@ -13956,7 +14085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11">
       <c r="A175">
         <v>174</v>
       </c>
@@ -13993,7 +14122,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11">
       <c r="A176">
         <v>175</v>
       </c>
@@ -14027,7 +14156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11">
       <c r="A177">
         <v>176</v>
       </c>
@@ -14064,7 +14193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11">
       <c r="A178">
         <v>177</v>
       </c>
@@ -14101,7 +14230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11">
       <c r="A179">
         <v>178</v>
       </c>
@@ -14138,7 +14267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11">
       <c r="A180">
         <v>179</v>
       </c>
@@ -14175,7 +14304,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11">
       <c r="A181">
         <v>180</v>
       </c>
@@ -14212,7 +14341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11">
       <c r="A182">
         <v>181</v>
       </c>
@@ -14246,7 +14375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11">
       <c r="A183">
         <v>182</v>
       </c>
@@ -14280,7 +14409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11">
       <c r="A184">
         <v>183</v>
       </c>
@@ -14317,7 +14446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11">
       <c r="A185">
         <v>184</v>
       </c>
@@ -14354,7 +14483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11">
       <c r="A186">
         <v>185</v>
       </c>
@@ -14391,7 +14520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11">
       <c r="A187">
         <v>186</v>
       </c>
@@ -14425,7 +14554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11">
       <c r="A188">
         <v>187</v>
       </c>
@@ -14459,7 +14588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11">
       <c r="A189">
         <v>188</v>
       </c>
@@ -14496,7 +14625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11">
       <c r="A190">
         <v>189</v>
       </c>
@@ -14533,7 +14662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11">
       <c r="A191">
         <v>190</v>
       </c>
@@ -14567,7 +14696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11">
       <c r="A192">
         <v>191</v>
       </c>
@@ -14604,7 +14733,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11">
       <c r="A193">
         <v>192</v>
       </c>
@@ -14641,7 +14770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11">
       <c r="A194">
         <v>193</v>
       </c>
@@ -14678,7 +14807,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11">
       <c r="A195">
         <v>194</v>
       </c>
@@ -14715,7 +14844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11">
       <c r="A196">
         <v>195</v>
       </c>
@@ -14752,7 +14881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11">
       <c r="A197">
         <v>196</v>
       </c>
@@ -14789,7 +14918,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11">
       <c r="A198">
         <v>197</v>
       </c>
@@ -14826,7 +14955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11">
       <c r="A199">
         <v>198</v>
       </c>
@@ -14863,7 +14992,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11">
       <c r="A200">
         <v>199</v>
       </c>
@@ -14900,7 +15029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11">
       <c r="A201">
         <v>200</v>
       </c>
@@ -14934,7 +15063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11">
       <c r="A202">
         <v>201</v>
       </c>
@@ -14971,7 +15100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11">
       <c r="A203">
         <v>202</v>
       </c>
@@ -15008,7 +15137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11">
       <c r="A204">
         <v>203</v>
       </c>
@@ -15045,7 +15174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11">
       <c r="A205">
         <v>204</v>
       </c>
@@ -15082,7 +15211,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11">
       <c r="A206">
         <v>205</v>
       </c>
@@ -15119,7 +15248,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11">
       <c r="A207">
         <v>206</v>
       </c>
@@ -15156,7 +15285,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11">
       <c r="A208">
         <v>207</v>
       </c>
@@ -15190,7 +15319,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11">
       <c r="A209">
         <v>208</v>
       </c>
@@ -15227,7 +15356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11">
       <c r="A210">
         <v>209</v>
       </c>
@@ -15264,7 +15393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11">
       <c r="A211">
         <v>210</v>
       </c>
@@ -15301,7 +15430,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11">
       <c r="A212">
         <v>211</v>
       </c>
@@ -15338,7 +15467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11">
       <c r="A213">
         <v>212</v>
       </c>
@@ -15375,7 +15504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11">
       <c r="A214">
         <v>213</v>
       </c>
@@ -15409,7 +15538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11">
       <c r="A215">
         <v>214</v>
       </c>
@@ -15443,7 +15572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11">
       <c r="A216">
         <v>215</v>
       </c>
@@ -15480,7 +15609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11">
       <c r="A217">
         <v>216</v>
       </c>
@@ -15517,7 +15646,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11">
       <c r="A218">
         <v>217</v>
       </c>
@@ -15554,7 +15683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11">
       <c r="A219">
         <v>218</v>
       </c>
@@ -15591,7 +15720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11">
       <c r="A220">
         <v>219</v>
       </c>
@@ -15628,7 +15757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11">
       <c r="A221">
         <v>220</v>
       </c>
@@ -15665,7 +15794,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11">
       <c r="A222">
         <v>221</v>
       </c>
@@ -15699,7 +15828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11">
       <c r="A223">
         <v>222</v>
       </c>
@@ -15736,7 +15865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11">
       <c r="A224">
         <v>223</v>
       </c>
@@ -15770,7 +15899,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11">
       <c r="A225">
         <v>224</v>
       </c>
@@ -15807,7 +15936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11">
       <c r="A226">
         <v>225</v>
       </c>
@@ -15844,7 +15973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11">
       <c r="A227">
         <v>226</v>
       </c>
@@ -15881,7 +16010,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11">
       <c r="A228">
         <v>227</v>
       </c>
@@ -15918,7 +16047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11">
       <c r="A229">
         <v>228</v>
       </c>
@@ -15955,7 +16084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11">
       <c r="A230">
         <v>229</v>
       </c>
@@ -15989,7 +16118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11">
       <c r="A231">
         <v>230</v>
       </c>
@@ -16026,7 +16155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11">
       <c r="A232">
         <v>231</v>
       </c>
@@ -16063,7 +16192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11">
       <c r="A233">
         <v>232</v>
       </c>
@@ -16100,7 +16229,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11">
       <c r="A234">
         <v>233</v>
       </c>
@@ -16137,7 +16266,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11">
       <c r="A235">
         <v>234</v>
       </c>
@@ -16174,7 +16303,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11">
       <c r="A236">
         <v>235</v>
       </c>
@@ -16211,7 +16340,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11">
       <c r="A237">
         <v>236</v>
       </c>
@@ -16245,7 +16374,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11">
       <c r="A238">
         <v>237</v>
       </c>
@@ -16282,7 +16411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11">
       <c r="A239">
         <v>238</v>
       </c>
@@ -16319,7 +16448,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11">
       <c r="A240">
         <v>239</v>
       </c>
@@ -16356,7 +16485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11">
       <c r="A241">
         <v>240</v>
       </c>
@@ -16390,7 +16519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11">
       <c r="A242">
         <v>241</v>
       </c>
@@ -16424,7 +16553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11">
       <c r="A243">
         <v>242</v>
       </c>
@@ -16458,7 +16587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11">
       <c r="A244">
         <v>243</v>
       </c>
@@ -16492,7 +16621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11">
       <c r="A245">
         <v>244</v>
       </c>
@@ -16529,7 +16658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11">
       <c r="A246">
         <v>245</v>
       </c>
@@ -16566,7 +16695,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11">
       <c r="A247">
         <v>246</v>
       </c>
@@ -16603,7 +16732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11">
       <c r="A248">
         <v>247</v>
       </c>
@@ -16640,7 +16769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11">
       <c r="A249">
         <v>248</v>
       </c>
@@ -16677,7 +16806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11">
       <c r="A250">
         <v>249</v>
       </c>
@@ -16714,7 +16843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11">
       <c r="A251">
         <v>250</v>
       </c>
@@ -16748,7 +16877,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11">
       <c r="A252">
         <v>251</v>
       </c>
@@ -16785,7 +16914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11">
       <c r="A253">
         <v>252</v>
       </c>
@@ -16822,7 +16951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11">
       <c r="A254">
         <v>253</v>
       </c>
@@ -16856,7 +16985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11">
       <c r="A255">
         <v>254</v>
       </c>
@@ -16893,7 +17022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11">
       <c r="A256">
         <v>255</v>
       </c>
@@ -16927,7 +17056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11">
       <c r="A257">
         <v>256</v>
       </c>
@@ -16964,7 +17093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11">
       <c r="A258">
         <v>257</v>
       </c>
@@ -17001,7 +17130,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11">
       <c r="A259">
         <v>258</v>
       </c>
@@ -17038,7 +17167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11">
       <c r="A260">
         <v>259</v>
       </c>
@@ -17075,7 +17204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11">
       <c r="A261">
         <v>260</v>
       </c>
@@ -17112,7 +17241,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11">
       <c r="A262">
         <v>261</v>
       </c>
@@ -17149,7 +17278,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11">
       <c r="A263">
         <v>262</v>
       </c>
@@ -17186,7 +17315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11">
       <c r="A264">
         <v>263</v>
       </c>
@@ -17223,7 +17352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11">
       <c r="A265">
         <v>264</v>
       </c>
@@ -17257,7 +17386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11">
       <c r="A266">
         <v>265</v>
       </c>
@@ -17294,7 +17423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11">
       <c r="A267">
         <v>266</v>
       </c>
@@ -17331,7 +17460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11">
       <c r="A268">
         <v>267</v>
       </c>
@@ -17368,7 +17497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11">
       <c r="A269">
         <v>268</v>
       </c>
@@ -17405,7 +17534,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11">
       <c r="A270">
         <v>269</v>
       </c>
@@ -17442,7 +17571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11">
       <c r="A271">
         <v>270</v>
       </c>
@@ -17479,7 +17608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11">
       <c r="A272">
         <v>271</v>
       </c>
@@ -17516,7 +17645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11">
       <c r="A273">
         <v>272</v>
       </c>
@@ -17550,7 +17679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11">
       <c r="A274">
         <v>273</v>
       </c>
@@ -17587,7 +17716,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11">
       <c r="A275">
         <v>274</v>
       </c>
@@ -17624,7 +17753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11">
       <c r="A276">
         <v>275</v>
       </c>
@@ -17661,7 +17790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11">
       <c r="A277">
         <v>276</v>
       </c>
@@ -17698,7 +17827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11">
       <c r="A278">
         <v>277</v>
       </c>
@@ -17735,7 +17864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11">
       <c r="A279">
         <v>278</v>
       </c>
@@ -17769,7 +17898,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11">
       <c r="A280">
         <v>279</v>
       </c>
@@ -17806,7 +17935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11">
       <c r="A281">
         <v>280</v>
       </c>
@@ -17840,7 +17969,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11">
       <c r="A282">
         <v>281</v>
       </c>
@@ -17877,7 +18006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11">
       <c r="A283">
         <v>282</v>
       </c>
@@ -17914,7 +18043,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11">
       <c r="A284">
         <v>283</v>
       </c>
@@ -17948,7 +18077,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11">
       <c r="A285">
         <v>284</v>
       </c>
@@ -17985,7 +18114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11">
       <c r="A286">
         <v>285</v>
       </c>
@@ -18019,7 +18148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11">
       <c r="A287">
         <v>286</v>
       </c>
@@ -18056,7 +18185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11">
       <c r="A288">
         <v>287</v>
       </c>
@@ -18090,7 +18219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11">
       <c r="A289">
         <v>288</v>
       </c>
@@ -18127,7 +18256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:11">
       <c r="A290">
         <v>289</v>
       </c>
@@ -18164,7 +18293,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11">
       <c r="A291">
         <v>290</v>
       </c>
@@ -18198,7 +18327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11">
       <c r="A292">
         <v>291</v>
       </c>
@@ -18235,7 +18364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:11">
       <c r="A293">
         <v>292</v>
       </c>
@@ -18272,7 +18401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:11">
       <c r="A294">
         <v>293</v>
       </c>
@@ -18309,7 +18438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:11">
       <c r="A295">
         <v>294</v>
       </c>
@@ -18346,7 +18475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:11">
       <c r="A296">
         <v>295</v>
       </c>
@@ -18383,7 +18512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:11">
       <c r="A297">
         <v>296</v>
       </c>
@@ -18420,7 +18549,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:11">
       <c r="A298">
         <v>297</v>
       </c>
@@ -18454,7 +18583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:11">
       <c r="A299">
         <v>298</v>
       </c>
@@ -18491,7 +18620,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:11">
       <c r="A300">
         <v>299</v>
       </c>
@@ -18528,7 +18657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:11">
       <c r="A301">
         <v>300</v>
       </c>
@@ -18571,13 +18700,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="20.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
@@ -18590,7 +18719,7 @@
     <col min="15" max="15" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>1045</v>
       </c>
@@ -18598,7 +18727,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
         <v>1049</v>
       </c>
@@ -18618,7 +18747,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -18634,7 +18763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -18652,7 +18781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -18670,7 +18799,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -18688,7 +18817,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -18706,7 +18835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -18724,7 +18853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -18742,7 +18871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -18757,8 +18886,11 @@
       <c r="F10" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="T10" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -18776,7 +18908,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -18794,7 +18926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -18812,7 +18944,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -18830,7 +18962,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20">
       <c r="A15" s="4" t="s">
         <v>1047</v>
       </c>
@@ -18840,7 +18972,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20">
       <c r="A16" s="4" t="s">
         <v>1048</v>
       </c>
@@ -18860,5 +18992,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>